<commit_message>
[tests] blinder les tests stocks
</commit_message>
<xml_diff>
--- a/web/fixtures/csv/test_data/carbure_template_simple_missing_data_cannot_validate.xlsx
+++ b/web/fixtures/csv/test_data/carbure_template_simple_missing_data_cannot_validate.xlsx
@@ -174,22 +174,22 @@
     <t xml:space="preserve">TEST2020FR0000609993</t>
   </si>
   <si>
+    <t xml:space="preserve">missing ETD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEST2020FR0000808981</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLIENTEU1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">520</t>
+  </si>
+  <si>
     <t xml:space="preserve">missing EP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TEST2020FR0000808981</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CLIENTEU1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">520</t>
-  </si>
-  <si>
-    <t xml:space="preserve">missing ETD</t>
   </si>
   <si>
     <t xml:space="preserve">JM</t>
@@ -2912,7 +2912,7 @@
   <dimension ref="A1:S10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="10:10"/>
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3508,7 +3508,7 @@
   <dimension ref="A1:B37"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="10:10 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3828,7 +3828,7 @@
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="10:10 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4020,7 +4020,7 @@
   <dimension ref="A1:B252"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="10:10 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6060,7 +6060,7 @@
   <dimension ref="A1:A54"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="10:10 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6354,7 +6354,7 @@
   <dimension ref="A1:C81"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="10:10 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
[tests] updated test suites
</commit_message>
<xml_diff>
--- a/web/fixtures/csv/test_data/carbure_template_simple_missing_data_cannot_validate.xlsx
+++ b/web/fixtures/csv/test_data/carbure_template_simple_missing_data_cannot_validate.xlsx
@@ -2909,10 +2909,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S10"/>
+  <dimension ref="A1:S12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="11:11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3489,6 +3489,7 @@
         <v>57</v>
       </c>
     </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -3508,7 +3509,7 @@
   <dimension ref="A1:B37"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="11:11 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3828,7 +3829,7 @@
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="11:11 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4020,7 +4021,7 @@
   <dimension ref="A1:B252"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="11:11 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6060,7 +6061,7 @@
   <dimension ref="A1:A54"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="11:11 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6354,7 +6355,7 @@
   <dimension ref="A1:C81"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="11:11 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>